<commit_message>
Site:Year:Treatment for most variables
</commit_message>
<xml_diff>
--- a/Data/SLA_Water Content_Final_May.xlsx
+++ b/Data/SLA_Water Content_Final_May.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/a_Resurrection/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B226A3-B305-5943-ACD9-6E34706F2E37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE52C0E-394C-0A49-A61F-BD1224A1325E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3931" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3929" uniqueCount="60">
   <si>
     <t>0.0698 or 0.0798</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -237,14 +237,6 @@
   </si>
   <si>
     <t>skip</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -729,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3081"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2308" zoomScale="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="E2312" sqref="E2312"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A926" zoomScale="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="E931" sqref="E931"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7171,7 +7163,7 @@
         <v>0.39</v>
       </c>
       <c r="E437" s="4">
-        <v>0.70799999999999996</v>
+        <v>7.0800000000000002E-2</v>
       </c>
       <c r="F437" s="9">
         <v>17.997</v>
@@ -8731,7 +8723,7 @@
         <v>0.2</v>
       </c>
       <c r="E515" s="4">
-        <v>0.35</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F515" s="9">
         <v>8.9730000000000008</v>
@@ -13351,7 +13343,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="F746" s="9">
-        <v>8439</v>
+        <v>8.4390000000000001</v>
       </c>
     </row>
     <row r="747" spans="1:6" x14ac:dyDescent="0.2">
@@ -15012,7 +15004,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
       <c r="F829" s="9">
-        <v>5661</v>
+        <v>5.6609999999999996</v>
       </c>
     </row>
     <row r="830" spans="1:6" x14ac:dyDescent="0.2">
@@ -17029,7 +17021,7 @@
         <v>0.36</v>
       </c>
       <c r="E930" s="4">
-        <v>1.099E-2</v>
+        <v>0.1099</v>
       </c>
       <c r="F930" s="9">
         <v>19.867000000000001</v>
@@ -18315,7 +18307,7 @@
         <v>7.3300000000000004E-2</v>
       </c>
       <c r="F994" s="9">
-        <v>1.008</v>
+        <v>11.007999999999999</v>
       </c>
     </row>
     <row r="995" spans="1:6" x14ac:dyDescent="0.2">
@@ -20458,7 +20450,7 @@
         <v>9.3200000000000005E-2</v>
       </c>
       <c r="F1101" s="9">
-        <v>1328</v>
+        <v>13.28</v>
       </c>
     </row>
     <row r="1102" spans="1:6" x14ac:dyDescent="0.2">
@@ -31705,7 +31697,7 @@
         <v>0.22</v>
       </c>
       <c r="E1779" s="10">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
       <c r="F1779" s="9">
         <v>9.2439999999999998</v>
@@ -34593,7 +34585,7 @@
         <v>0.22</v>
       </c>
       <c r="E1924" s="10">
-        <v>0.67500000000000004</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="F1924" s="9">
         <v>9.3089999999999993</v>
@@ -36730,7 +36722,7 @@
         <v>0.48</v>
       </c>
       <c r="E2031" s="4">
-        <v>1.18E-2</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="F2031" s="9">
         <v>21.344999999999999</v>
@@ -42845,9 +42837,7 @@
       <c r="C2337" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2337" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="D2337" s="4"/>
       <c r="E2337" s="4"/>
       <c r="F2337" s="9"/>
       <c r="G2337" s="4" t="s">
@@ -43308,7 +43298,7 @@
       <c r="E2360" s="4"/>
       <c r="F2360" s="9"/>
       <c r="G2360" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2361" spans="1:7" x14ac:dyDescent="0.2">
@@ -43347,7 +43337,7 @@
       <c r="E2362" s="4"/>
       <c r="F2362" s="9"/>
       <c r="G2362" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2363" spans="1:7" x14ac:dyDescent="0.2">
@@ -44047,7 +44037,7 @@
       <c r="E2397" s="16"/>
       <c r="F2397" s="15"/>
       <c r="G2397" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2398" spans="1:7" x14ac:dyDescent="0.2">
@@ -44064,7 +44054,7 @@
       <c r="E2398" s="4"/>
       <c r="F2398" s="9"/>
       <c r="G2398" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2399" spans="1:7" x14ac:dyDescent="0.2">
@@ -44621,7 +44611,7 @@
       <c r="E2426" s="4"/>
       <c r="F2426" s="9"/>
       <c r="G2426" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2427" spans="1:7" x14ac:dyDescent="0.2">
@@ -45502,7 +45492,7 @@
       <c r="E2470" s="4"/>
       <c r="F2470" s="9"/>
       <c r="G2470" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2471" spans="1:7" x14ac:dyDescent="0.2">
@@ -45939,7 +45929,7 @@
       <c r="E2492" s="4"/>
       <c r="F2492" s="9"/>
       <c r="G2492" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2493" spans="1:7" x14ac:dyDescent="0.2">
@@ -46176,7 +46166,7 @@
       <c r="E2504" s="4"/>
       <c r="F2504" s="9"/>
       <c r="G2504" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2505" spans="1:7" x14ac:dyDescent="0.2">
@@ -46629,13 +46619,11 @@
       <c r="C2527" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2527" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="D2527" s="4"/>
       <c r="E2527" s="4"/>
       <c r="F2527" s="9"/>
       <c r="G2527" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2528" spans="1:7" x14ac:dyDescent="0.2">
@@ -46852,7 +46840,7 @@
       <c r="E2538" s="4"/>
       <c r="F2538" s="9"/>
       <c r="G2538" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2539" spans="1:7" x14ac:dyDescent="0.2">
@@ -47269,7 +47257,7 @@
       <c r="E2559" s="4"/>
       <c r="F2559" s="9"/>
       <c r="G2559" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2560" spans="1:7" x14ac:dyDescent="0.2">
@@ -52847,7 +52835,7 @@
         <v>20</v>
       </c>
       <c r="D2840" s="4">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="E2840" s="4">
         <v>6.0999999999999999E-2</v>

</xml_diff>